<commit_message>
modified exl and material files
</commit_message>
<xml_diff>
--- a/exl.xlsx
+++ b/exl.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanjay\Desktop\xman\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{522E1652-5887-4A07-82F5-FA30BD5E75DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF40073-8D76-471D-9CCB-5B8649686DEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,9 +26,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>env=dev</t>
+  </si>
+  <si>
+    <t>url="www.myapplication.com"</t>
   </si>
 </sst>
 </file>
@@ -346,10 +349,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -395,6 +398,14 @@
       </c>
       <c r="B8" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>